<commit_message>
making simpler tests with charging station
</commit_message>
<xml_diff>
--- a/output/df_con_electric.xlsx
+++ b/output/df_con_electric.xlsx
@@ -14,24 +14,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
-  <si>
-    <t>net1</t>
-  </si>
-  <si>
-    <t>pv1</t>
-  </si>
-  <si>
-    <t>bat1</t>
-  </si>
-  <si>
-    <t>CHP1</t>
-  </si>
-  <si>
-    <t>pvt1</t>
-  </si>
-  <si>
-    <t>demand1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>P_from_net1</t>
+  </si>
+  <si>
+    <t>P_from_pv1</t>
+  </si>
+  <si>
+    <t>P_from_bat1</t>
+  </si>
+  <si>
+    <t>P_from_CHP1</t>
+  </si>
+  <si>
+    <t>P_from_pvt1</t>
+  </si>
+  <si>
+    <t>P_to_demand1</t>
+  </si>
+  <si>
+    <t>P_to_net1</t>
+  </si>
+  <si>
+    <t>P_to_bat1</t>
+  </si>
+  <si>
+    <t>P_net1_demand1</t>
+  </si>
+  <si>
+    <t>P_pv1_demand1</t>
+  </si>
+  <si>
+    <t>P_pv1_net1</t>
+  </si>
+  <si>
+    <t>P_pv1_bat1</t>
+  </si>
+  <si>
+    <t>P_bat1_demand1</t>
+  </si>
+  <si>
+    <t>P_bat1_net1</t>
+  </si>
+  <si>
+    <t>P_CHP1_demand1</t>
+  </si>
+  <si>
+    <t>P_CHP1_net1</t>
+  </si>
+  <si>
+    <t>P_CHP1_bat1</t>
+  </si>
+  <si>
+    <t>P_pvt1_demand1</t>
+  </si>
+  <si>
+    <t>P_pvt1_net1</t>
+  </si>
+  <si>
+    <t>P_pvt1_bat1</t>
   </si>
 </sst>
 </file>
@@ -416,60 +458,60 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving before receiding horizon attempt
</commit_message>
<xml_diff>
--- a/output/df_con_electric.xlsx
+++ b/output/df_con_electric.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>P_from_net1</t>
   </si>
@@ -82,9 +82,6 @@
     <t>P_pv1_charging_station2</t>
   </si>
   <si>
-    <t>P_pv1_heat_pump1</t>
-  </si>
-  <si>
     <t>P_bat1_demand1</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>P_bat1_charging_station2</t>
   </si>
   <si>
-    <t>P_bat1_heat_pump1</t>
-  </si>
-  <si>
     <t>P_CHP1_demand1</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>P_CHP1_charging_station2</t>
   </si>
   <si>
-    <t>P_CHP1_heat_pump1</t>
-  </si>
-  <si>
     <t>P_pvt1_demand1</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
   </si>
   <si>
     <t>P_pvt1_charging_station2</t>
-  </si>
-  <si>
-    <t>P_pvt1_heat_pump1</t>
   </si>
 </sst>
 </file>
@@ -528,13 +516,13 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -551,13 +539,13 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -577,10 +565,10 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -597,13 +585,13 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -620,13 +608,13 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -639,17 +627,17 @@
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>

</xml_diff>